<commit_message>
Update D score categories and intervals.xlsx
</commit_message>
<xml_diff>
--- a/code/analysis/D score categories and intervals.xlsx
+++ b/code/analysis/D score categories and intervals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/comparing-implicit-measure-cis/code/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9746B783-E6E4-BE4F-8D32-5D1E16D70E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0CCCBF-5F12-A94D-898A-A4E938732C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="1080" windowWidth="28040" windowHeight="17440" xr2:uid="{717A163C-019E-3F4F-8160-90DAA1A70CB2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>measure</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Predicted 95% CI</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>D score cutoffs were extracted from the IAT code employed on project implicit that gives feedback to participants. The predicted 95% CI is taken from our current results, ie the predicted 95% interval for that D score for each domain. See analysis_iat_D.html and analysis_iat_D.Rmd</t>
   </si>
 </sst>
 </file>
@@ -197,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -217,6 +223,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DB31E1-4BF9-1746-9196-026A0E065DFF}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -546,10 +555,12 @@
     <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" style="7" customWidth="1"/>
     <col min="6" max="6" width="50" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="73.83203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34">
+    <row r="1" spans="1:8" ht="34">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -568,8 +579,11 @@
       <c r="F1" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="68">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -588,8 +602,11 @@
       <c r="F2" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -609,7 +626,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -629,7 +646,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -649,7 +666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -669,7 +686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -689,7 +706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -709,7 +726,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -729,7 +746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -749,7 +766,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -769,7 +786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -789,7 +806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>